<commit_message>
Added more countries with Trues.
</commit_message>
<xml_diff>
--- a/raw_text_input.xlsx
+++ b/raw_text_input.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="z0tqnY8Pv6VEjdB05YDFp9F3uPmqyz7Ac93TEHStJsk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Ax8g4N8O5W5YlP1blm5wDDB3cu/XqlWmUVHybPnFhdM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>RAW_TEXT</t>
   </si>
@@ -56,15 +56,8 @@
 Download Now
 If you do not take action, your personal data will be compromised.
 Sincerely,
-UVic Support Team</t>
-  </si>
-  <si>
-    <t>Subject: Immediate Payment Required to Avoid Legal Action
-Dear John,
-You have an outstanding tax balance of $2,400 that must be paid immediately. Failure to comply will result in legal action, including wage garnishment and property seizure. To resolve this matter, please call us at [Fake Phone Number] or click the payment link below:
-Pay Now
-Sincerely,
-Internal Revenue Service (IRS)</t>
+UVic Support Team
+Slovakia</t>
   </si>
   <si>
     <t>Subject: I Think I’ve Found My Soulmate
@@ -89,12 +82,18 @@
   <si>
     <t>Dan</t>
   </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -109,6 +108,11 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -150,6 +154,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -399,7 +406,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -419,10 +426,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -444,20 +451,29 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -1437,7 +1453,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>